<commit_message>
Fix level 4 and complete level 6
</commit_message>
<xml_diff>
--- a/Base/TileMap/Formatting/Level6.xlsx
+++ b/Base/TileMap/Formatting/Level6.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Level8" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -556,414 +555,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1353,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AP31" sqref="AP31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1800,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="R3" s="1">
         <v>1</v>
@@ -1824,7 +1416,7 @@
         <v>1</v>
       </c>
       <c r="Y3" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Z3" s="1">
         <v>1</v>
@@ -1848,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="AG3" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AH3" s="1">
         <v>1</v>
@@ -2293,7 +1885,7 @@
         <v>1</v>
       </c>
       <c r="AZ5" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="BA5" s="1">
         <v>0</v>
@@ -2863,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="AV8" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="AW8" s="1">
         <v>0</v>
@@ -2902,7 +2494,7 @@
         <v>0</v>
       </c>
       <c r="BI8" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="BJ8" s="1">
         <v>1</v>
@@ -3096,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="BI9" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="BJ9" s="1">
         <v>1</v>
@@ -3704,7 +3296,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -3818,7 +3410,7 @@
         <v>0</v>
       </c>
       <c r="AQ13" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AR13" s="1">
         <v>1</v>
@@ -3946,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="U14" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="V14" s="1">
         <v>0</v>
@@ -4227,7 +3819,7 @@
         <v>0</v>
       </c>
       <c r="AX15" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AY15" s="1">
         <v>1</v>
@@ -4627,7 +4219,7 @@
         <v>1</v>
       </c>
       <c r="BB17" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="BC17" s="1">
         <v>1</v>
@@ -4925,7 +4517,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Y19" s="1">
         <v>0</v>
@@ -5027,7 +4619,7 @@
         <v>0</v>
       </c>
       <c r="BF19" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="BG19" s="1">
         <v>0</v>
@@ -5256,7 +4848,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -5271,7 +4863,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="K21" s="1">
         <v>0</v>
@@ -5355,7 +4947,7 @@
         <v>0</v>
       </c>
       <c r="AL21" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AM21" s="1">
         <v>1</v>
@@ -5370,7 +4962,7 @@
         <v>0</v>
       </c>
       <c r="AQ21" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AR21" s="1">
         <v>1</v>
@@ -5427,7 +5019,7 @@
         <v>1</v>
       </c>
       <c r="BJ21" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="BK21" s="1">
         <v>0</v>
@@ -5498,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="U22" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="V22" s="1">
         <v>17</v>
@@ -5516,7 +5108,7 @@
         <v>15</v>
       </c>
       <c r="AA22" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AB22" s="1">
         <v>0</v>
@@ -6089,7 +5681,7 @@
         <v>0</v>
       </c>
       <c r="X25" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Y25" s="1">
         <v>0</v>
@@ -6185,7 +5777,7 @@
         <v>1</v>
       </c>
       <c r="BD25" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="BE25" s="1">
         <v>0</v>
@@ -6253,7 +5845,7 @@
         <v>1</v>
       </c>
       <c r="N26" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="O26" s="1">
         <v>17</v>
@@ -6808,7 +6400,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -6922,7 +6514,7 @@
         <v>0</v>
       </c>
       <c r="AQ29" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AR29" s="1">
         <v>1</v>
@@ -6934,7 +6526,7 @@
         <v>0</v>
       </c>
       <c r="AU29" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AV29" s="1">
         <v>1</v>
@@ -6964,7 +6556,7 @@
         <v>1</v>
       </c>
       <c r="BE29" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="BF29" s="1">
         <v>1</v>
@@ -7534,7 +7126,7 @@
         <v>0</v>
       </c>
       <c r="BA32" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="BB32" s="1">
         <v>0</v>
@@ -7549,7 +7141,7 @@
         <v>0</v>
       </c>
       <c r="BF32" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="BG32" s="1">
         <v>0</v>
@@ -7728,7 +7320,7 @@
         <v>0</v>
       </c>
       <c r="BA33" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="BB33" s="1">
         <v>0</v>
@@ -7737,7 +7329,7 @@
         <v>1</v>
       </c>
       <c r="BD33" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="BE33" s="1">
         <v>0</v>
@@ -7835,7 +7427,7 @@
         <v>0</v>
       </c>
       <c r="X34" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Y34" s="1">
         <v>0</v>
@@ -8032,7 +7624,7 @@
         <v>0</v>
       </c>
       <c r="Y35" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Z35" s="1">
         <v>0</v>
@@ -8295,7 +7887,7 @@
         <v>1</v>
       </c>
       <c r="AV36" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="AW36" s="1">
         <v>0</v>
@@ -8704,7 +8296,7 @@
         <v>0</v>
       </c>
       <c r="BC38" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="BD38" s="1">
         <v>1</v>
@@ -9172,7 +8764,7 @@
         <v>1</v>
       </c>
       <c r="Q41" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="R41" s="1">
         <v>1</v>
@@ -9196,7 +8788,7 @@
         <v>1</v>
       </c>
       <c r="Y41" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="Z41" s="1">
         <v>1</v>
@@ -9220,7 +8812,7 @@
         <v>1</v>
       </c>
       <c r="AG41" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AH41" s="1">
         <v>1</v>
@@ -11258,53 +10850,53 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="55" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="between">
       <formula>15</formula>
       <formula>18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:BL51">
-    <cfRule type="cellIs" dxfId="52" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:Y18 V16:AC16 S16:T16">
-    <cfRule type="cellIs" dxfId="51" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="between">
       <formula>15</formula>
       <formula>18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U16:Y18 V16:AC16 S16:T16">
-    <cfRule type="cellIs" dxfId="48" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U17:U25 V19:AA19 AA20:AA25 K21:T21 Q23:T23 Q24:R30 H7:J21 H27:Q31 T22:T26 T18:T20 U18:AB18 AB19:AB26 U26:AA26 R16:R27 Q14:AF14 AF15:AF30 P30:AE30 P15:P29 O12:AH12 N13:N32 O32:AH32 AH13:AH31 K11:L35 M34:AK35 AJ10:AK33 K7:Q20 W6:W18">
-    <cfRule type="cellIs" dxfId="47" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
       <formula>15</formula>
       <formula>18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U17:U25 V19:AA19 AA20:AA25 K21:T21 Q23:T23 Q24:R30 H7:J21 H27:Q31 T22:T26 T18:T20 U18:AB18 AB19:AB26 U26:AA26 R16:R27 Q14:AF14 AF15:AF30 P30:AE30 P15:P29 O12:AH12 N13:N32 O32:AH32 AH13:AH31 K11:L35 M34:AK35 AJ10:AK33 K7:Q20 W6:W18">
-    <cfRule type="cellIs" dxfId="44" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>